<commit_message>
Annual data availability of data sources and year splits for census
</commit_message>
<xml_diff>
--- a/data/misc/Data_sources_years.xlsx
+++ b/data/misc/Data_sources_years.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SHIVANI\MEngCEM\UTTRI\RA Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP USER\Documents\repos\thesis\data\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34C1819F-E31C-4D2E-9ABE-3FA62F6B96DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F97121F-FCAE-4A9B-A626-DEB43D50EFCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2409B5E1-C8AF-4D99-A624-F0DB51F6EDE7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22224" windowHeight="13176" xr2:uid="{2409B5E1-C8AF-4D99-A624-F0DB51F6EDE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -159,11 +159,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -175,11 +308,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -200,7 +329,64 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -528,580 +714,580 @@
   <dimension ref="A1:AV9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="5" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="15" width="5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="26" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="15" width="5" style="5" customWidth="1"/>
     <col min="16" max="48" width="5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="16">
         <v>1971</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1" s="17">
         <v>1972</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="18">
         <v>1973</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1" s="16">
         <v>1974</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F1" s="17">
         <v>1975</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="17">
         <v>1976</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1" s="17">
         <v>1977</v>
       </c>
-      <c r="I1" s="5">
+      <c r="I1" s="18">
         <v>1978</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="16">
         <v>1979</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K1" s="17">
         <v>1980</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="17">
         <v>1981</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="17">
         <v>1982</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N1" s="18">
         <v>1983</v>
       </c>
-      <c r="O1" s="5">
+      <c r="O1" s="16">
         <v>1984</v>
       </c>
-      <c r="P1" s="5">
+      <c r="P1" s="17">
         <v>1985</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="Q1" s="17">
         <v>1986</v>
       </c>
-      <c r="R1" s="5">
+      <c r="R1" s="17">
         <v>1987</v>
       </c>
-      <c r="S1" s="5">
+      <c r="S1" s="18">
         <v>1988</v>
       </c>
-      <c r="T1" s="5">
+      <c r="T1" s="16">
         <v>1989</v>
       </c>
-      <c r="U1" s="5">
+      <c r="U1" s="17">
         <v>1990</v>
       </c>
-      <c r="V1" s="5">
+      <c r="V1" s="17">
         <v>1991</v>
       </c>
-      <c r="W1" s="5">
+      <c r="W1" s="17">
         <v>1992</v>
       </c>
-      <c r="X1" s="5">
+      <c r="X1" s="18">
         <v>1993</v>
       </c>
-      <c r="Y1" s="5">
+      <c r="Y1" s="16">
         <v>1994</v>
       </c>
-      <c r="Z1" s="5">
+      <c r="Z1" s="17">
         <v>1995</v>
       </c>
-      <c r="AA1" s="5">
+      <c r="AA1" s="17">
         <v>1996</v>
       </c>
-      <c r="AB1" s="5">
+      <c r="AB1" s="17">
         <v>1997</v>
       </c>
-      <c r="AC1" s="5">
+      <c r="AC1" s="18">
         <v>1998</v>
       </c>
-      <c r="AD1" s="5">
+      <c r="AD1" s="16">
         <v>1999</v>
       </c>
-      <c r="AE1" s="5">
+      <c r="AE1" s="17">
         <v>2000</v>
       </c>
-      <c r="AF1" s="5">
+      <c r="AF1" s="17">
         <v>2001</v>
       </c>
-      <c r="AG1" s="5">
+      <c r="AG1" s="17">
         <v>2002</v>
       </c>
-      <c r="AH1" s="5">
+      <c r="AH1" s="18">
         <v>2003</v>
       </c>
-      <c r="AI1" s="5">
+      <c r="AI1" s="16">
         <v>2004</v>
       </c>
-      <c r="AJ1" s="5">
+      <c r="AJ1" s="17">
         <v>2005</v>
       </c>
-      <c r="AK1" s="5">
+      <c r="AK1" s="17">
         <v>2006</v>
       </c>
-      <c r="AL1" s="5">
+      <c r="AL1" s="17">
         <v>2007</v>
       </c>
-      <c r="AM1" s="5">
+      <c r="AM1" s="18">
         <v>2008</v>
       </c>
-      <c r="AN1" s="5">
+      <c r="AN1" s="16">
         <v>2009</v>
       </c>
-      <c r="AO1" s="5">
+      <c r="AO1" s="17">
         <v>2010</v>
       </c>
-      <c r="AP1" s="5">
+      <c r="AP1" s="17">
         <v>2011</v>
       </c>
-      <c r="AQ1" s="5">
+      <c r="AQ1" s="17">
         <v>2012</v>
       </c>
-      <c r="AR1" s="5">
+      <c r="AR1" s="18">
         <v>2013</v>
       </c>
-      <c r="AS1" s="5">
+      <c r="AS1" s="16">
         <v>2014</v>
       </c>
-      <c r="AT1" s="5">
+      <c r="AT1" s="17">
         <v>2015</v>
       </c>
-      <c r="AU1" s="5">
+      <c r="AU1" s="17">
         <v>2016</v>
       </c>
-      <c r="AV1" s="5">
+      <c r="AV1" s="18">
         <v>2017</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="19"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="9"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="9"/>
+      <c r="L2" s="7"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="21"/>
       <c r="P2" s="2"/>
-      <c r="Q2" s="8"/>
+      <c r="Q2" s="6"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="31"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="8"/>
+      <c r="V2" s="6"/>
       <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="31"/>
       <c r="Z2" s="2"/>
-      <c r="AA2" s="8"/>
+      <c r="AA2" s="6"/>
       <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="31"/>
       <c r="AE2" s="2"/>
-      <c r="AF2" s="8"/>
+      <c r="AF2" s="6"/>
       <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="31"/>
       <c r="AJ2" s="2"/>
-      <c r="AK2" s="8"/>
+      <c r="AK2" s="6"/>
       <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="31"/>
       <c r="AO2" s="2"/>
-      <c r="AP2" s="8"/>
+      <c r="AP2" s="6"/>
       <c r="AQ2" s="2"/>
-      <c r="AR2" s="2"/>
-      <c r="AS2" s="2"/>
+      <c r="AR2" s="28"/>
+      <c r="AS2" s="31"/>
       <c r="AT2" s="2"/>
-      <c r="AU2" s="8"/>
-      <c r="AV2" s="2"/>
+      <c r="AU2" s="6"/>
+      <c r="AV2" s="28"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="21"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="12"/>
+      <c r="Q3" s="10"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="31"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="12"/>
+      <c r="V3" s="10"/>
       <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="31"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="12"/>
+      <c r="AA3" s="10"/>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="31"/>
       <c r="AE3" s="2"/>
-      <c r="AF3" s="12"/>
+      <c r="AF3" s="10"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="31"/>
       <c r="AJ3" s="2"/>
-      <c r="AK3" s="12"/>
+      <c r="AK3" s="10"/>
       <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
+      <c r="AM3" s="28"/>
+      <c r="AN3" s="31"/>
       <c r="AO3" s="2"/>
-      <c r="AP3" s="12"/>
+      <c r="AP3" s="10"/>
       <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
+      <c r="AR3" s="28"/>
+      <c r="AS3" s="31"/>
       <c r="AT3" s="2"/>
-      <c r="AU3" s="12"/>
-      <c r="AV3" s="2"/>
+      <c r="AU3" s="10"/>
+      <c r="AV3" s="28"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="21"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="31"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="31"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="31"/>
       <c r="AE4" s="2"/>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="13"/>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="13"/>
-      <c r="AJ4" s="13"/>
-      <c r="AK4" s="13"/>
-      <c r="AL4" s="13"/>
-      <c r="AM4" s="13"/>
-      <c r="AN4" s="13"/>
-      <c r="AO4" s="13"/>
-      <c r="AP4" s="13"/>
-      <c r="AQ4" s="13"/>
-      <c r="AR4" s="13"/>
-      <c r="AS4" s="13"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="33"/>
+      <c r="AI4" s="36"/>
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="11"/>
+      <c r="AL4" s="11"/>
+      <c r="AM4" s="33"/>
+      <c r="AN4" s="36"/>
+      <c r="AO4" s="11"/>
+      <c r="AP4" s="11"/>
+      <c r="AQ4" s="11"/>
+      <c r="AR4" s="33"/>
+      <c r="AS4" s="36"/>
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
-      <c r="AV4" s="2"/>
+      <c r="AV4" s="28"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="21"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="31"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="31"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="31"/>
       <c r="AE5" s="2"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="15"/>
-      <c r="AL5" s="15"/>
-      <c r="AM5" s="15"/>
-      <c r="AN5" s="15"/>
-      <c r="AO5" s="15"/>
-      <c r="AP5" s="15"/>
-      <c r="AQ5" s="15"/>
-      <c r="AR5" s="15"/>
-      <c r="AS5" s="15"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="34"/>
+      <c r="AI5" s="37"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="34"/>
+      <c r="AN5" s="37"/>
+      <c r="AO5" s="13"/>
+      <c r="AP5" s="13"/>
+      <c r="AQ5" s="13"/>
+      <c r="AR5" s="34"/>
+      <c r="AS5" s="37"/>
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
-      <c r="AV5" s="2"/>
+      <c r="AV5" s="28"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="21"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="31"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="31"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="31"/>
       <c r="AE6" s="2"/>
-      <c r="AF6" s="14"/>
-      <c r="AG6" s="14"/>
-      <c r="AH6" s="14"/>
-      <c r="AI6" s="14"/>
-      <c r="AJ6" s="14"/>
-      <c r="AK6" s="14"/>
-      <c r="AL6" s="14"/>
-      <c r="AM6" s="14"/>
-      <c r="AN6" s="14"/>
-      <c r="AO6" s="14"/>
-      <c r="AP6" s="14"/>
-      <c r="AQ6" s="14"/>
-      <c r="AR6" s="14"/>
-      <c r="AS6" s="2"/>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="35"/>
+      <c r="AI6" s="38"/>
+      <c r="AJ6" s="12"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="12"/>
+      <c r="AM6" s="35"/>
+      <c r="AN6" s="38"/>
+      <c r="AO6" s="12"/>
+      <c r="AP6" s="12"/>
+      <c r="AQ6" s="12"/>
+      <c r="AR6" s="35"/>
+      <c r="AS6" s="31"/>
       <c r="AT6" s="2"/>
       <c r="AU6" s="2"/>
-      <c r="AV6" s="2"/>
+      <c r="AV6" s="28"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="10"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="21"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="10"/>
+      <c r="L7" s="8"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="21"/>
       <c r="P7" s="2"/>
-      <c r="Q7" s="11"/>
+      <c r="Q7" s="9"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="31"/>
       <c r="U7" s="2"/>
-      <c r="V7" s="11"/>
+      <c r="V7" s="9"/>
       <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="31"/>
       <c r="Z7" s="2"/>
-      <c r="AA7" s="11"/>
+      <c r="AA7" s="9"/>
       <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="31"/>
       <c r="AE7" s="2"/>
-      <c r="AF7" s="11"/>
+      <c r="AF7" s="9"/>
       <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
+      <c r="AH7" s="28"/>
+      <c r="AI7" s="31"/>
       <c r="AJ7" s="2"/>
-      <c r="AK7" s="11"/>
+      <c r="AK7" s="9"/>
       <c r="AL7" s="2"/>
-      <c r="AM7" s="2"/>
-      <c r="AN7" s="2"/>
+      <c r="AM7" s="28"/>
+      <c r="AN7" s="31"/>
       <c r="AO7" s="2"/>
-      <c r="AP7" s="11"/>
+      <c r="AP7" s="9"/>
       <c r="AQ7" s="2"/>
-      <c r="AR7" s="2"/>
-      <c r="AS7" s="2"/>
+      <c r="AR7" s="28"/>
+      <c r="AS7" s="31"/>
       <c r="AT7" s="2"/>
-      <c r="AU7" s="11"/>
-      <c r="AV7" s="2"/>
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="28"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="23"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="23"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="23"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="23"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="23"/>
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
+      <c r="AH8" s="24"/>
+      <c r="AI8" s="23"/>
       <c r="AJ8" s="3"/>
       <c r="AK8" s="3"/>
       <c r="AL8" s="3"/>
-      <c r="AM8" s="3"/>
-      <c r="AN8" s="3"/>
+      <c r="AM8" s="24"/>
+      <c r="AN8" s="23"/>
       <c r="AO8" s="3"/>
       <c r="AP8" s="3"/>
       <c r="AQ8" s="3"/>
-      <c r="AR8" s="3"/>
-      <c r="AS8" s="3"/>
+      <c r="AR8" s="24"/>
+      <c r="AS8" s="23"/>
       <c r="AT8" s="3"/>
       <c r="AU8" s="3"/>
-      <c r="AV8" s="3"/>
+      <c r="AV8" s="24"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
-      <c r="AF9" s="2"/>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2"/>
-      <c r="AI9" s="2"/>
-      <c r="AJ9" s="2"/>
-      <c r="AK9" s="2"/>
-      <c r="AL9" s="2"/>
-      <c r="AM9" s="2"/>
-      <c r="AN9" s="2"/>
-      <c r="AO9" s="2"/>
-      <c r="AP9" s="16"/>
-      <c r="AQ9" s="2"/>
-      <c r="AR9" s="2"/>
-      <c r="AS9" s="2"/>
-      <c r="AT9" s="2"/>
-      <c r="AU9" s="2"/>
-      <c r="AV9" s="2"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="30"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="29"/>
+      <c r="AC9" s="30"/>
+      <c r="AD9" s="32"/>
+      <c r="AE9" s="29"/>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="29"/>
+      <c r="AH9" s="30"/>
+      <c r="AI9" s="32"/>
+      <c r="AJ9" s="29"/>
+      <c r="AK9" s="29"/>
+      <c r="AL9" s="29"/>
+      <c r="AM9" s="30"/>
+      <c r="AN9" s="32"/>
+      <c r="AO9" s="29"/>
+      <c r="AP9" s="39"/>
+      <c r="AQ9" s="29"/>
+      <c r="AR9" s="30"/>
+      <c r="AS9" s="32"/>
+      <c r="AT9" s="29"/>
+      <c r="AU9" s="29"/>
+      <c r="AV9" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add Fuel prices in Toronto, color sources by groups
</commit_message>
<xml_diff>
--- a/data/misc/Data_sources_years.xlsx
+++ b/data/misc/Data_sources_years.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP USER\Documents\repos\thesis\data\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F97121F-FCAE-4A9B-A626-DEB43D50EFCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C55B2F-33EC-4846-83CC-C578C61F2E0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22224" windowHeight="13176" xr2:uid="{2409B5E1-C8AF-4D99-A624-F0DB51F6EDE7}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>DMTI land use</t>
   </si>
@@ -58,6 +58,9 @@
   <si>
     <t>TTS (2001 zone system)</t>
   </si>
+  <si>
+    <t>Fuel price in Toronto</t>
+  </si>
 </sst>
 </file>
 
@@ -80,7 +83,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +138,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -296,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -387,6 +396,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D36D5B-2CC9-4B45-8386-8C93BA53E55C}">
-  <dimension ref="A1:AV9"/>
+  <dimension ref="A1:AV10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,6 +1302,18 @@
       <c r="AU9" s="29"/>
       <c r="AV9" s="30"/>
     </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="AA10" s="41"/>
+      <c r="AF10" s="41"/>
+      <c r="AK10" s="41"/>
+      <c r="AP10" s="41"/>
+      <c r="AU10" s="41"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
termporal spans of data sources
</commit_message>
<xml_diff>
--- a/data/misc/Data_sources_years.xlsx
+++ b/data/misc/Data_sources_years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP USER\Documents\repos\thesis\data\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C55B2F-33EC-4846-83CC-C578C61F2E0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAD52CE-8937-4502-AE6C-0884E43AD4FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22224" windowHeight="13176" xr2:uid="{2409B5E1-C8AF-4D99-A624-F0DB51F6EDE7}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,8 +82,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,8 +151,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -257,6 +282,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -266,9 +302,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -281,9 +315,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -294,6 +326,75 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -305,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -339,7 +440,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -359,49 +459,69 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,6 +530,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99FF"/>
       <color rgb="FF9933FF"/>
       <color rgb="FFFF9933"/>
       <color rgb="FFCC6600"/>
@@ -726,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D36D5B-2CC9-4B45-8386-8C93BA53E55C}">
   <dimension ref="A1:AV10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="BB5" sqref="BB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,575 +865,615 @@
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16">
+      <c r="B1" s="15">
         <v>1971</v>
       </c>
-      <c r="C1" s="17">
+      <c r="C1" s="16">
         <v>1972</v>
       </c>
-      <c r="D1" s="18">
+      <c r="D1" s="17">
         <v>1973</v>
       </c>
-      <c r="E1" s="16">
+      <c r="E1" s="15">
         <v>1974</v>
       </c>
-      <c r="F1" s="17">
+      <c r="F1" s="16">
         <v>1975</v>
       </c>
-      <c r="G1" s="17">
+      <c r="G1" s="16">
         <v>1976</v>
       </c>
-      <c r="H1" s="17">
+      <c r="H1" s="16">
         <v>1977</v>
       </c>
-      <c r="I1" s="18">
+      <c r="I1" s="17">
         <v>1978</v>
       </c>
-      <c r="J1" s="16">
+      <c r="J1" s="15">
         <v>1979</v>
       </c>
-      <c r="K1" s="17">
+      <c r="K1" s="16">
         <v>1980</v>
       </c>
-      <c r="L1" s="17">
+      <c r="L1" s="16">
         <v>1981</v>
       </c>
-      <c r="M1" s="17">
+      <c r="M1" s="16">
         <v>1982</v>
       </c>
-      <c r="N1" s="18">
+      <c r="N1" s="17">
         <v>1983</v>
       </c>
-      <c r="O1" s="16">
+      <c r="O1" s="15">
         <v>1984</v>
       </c>
-      <c r="P1" s="17">
+      <c r="P1" s="16">
         <v>1985</v>
       </c>
-      <c r="Q1" s="17">
+      <c r="Q1" s="16">
         <v>1986</v>
       </c>
-      <c r="R1" s="17">
+      <c r="R1" s="16">
         <v>1987</v>
       </c>
-      <c r="S1" s="18">
+      <c r="S1" s="17">
         <v>1988</v>
       </c>
-      <c r="T1" s="16">
+      <c r="T1" s="15">
         <v>1989</v>
       </c>
-      <c r="U1" s="17">
+      <c r="U1" s="16">
         <v>1990</v>
       </c>
-      <c r="V1" s="17">
+      <c r="V1" s="16">
         <v>1991</v>
       </c>
-      <c r="W1" s="17">
+      <c r="W1" s="16">
         <v>1992</v>
       </c>
-      <c r="X1" s="18">
+      <c r="X1" s="17">
         <v>1993</v>
       </c>
-      <c r="Y1" s="16">
+      <c r="Y1" s="15">
         <v>1994</v>
       </c>
-      <c r="Z1" s="17">
+      <c r="Z1" s="16">
         <v>1995</v>
       </c>
-      <c r="AA1" s="17">
+      <c r="AA1" s="16">
         <v>1996</v>
       </c>
-      <c r="AB1" s="17">
+      <c r="AB1" s="16">
         <v>1997</v>
       </c>
-      <c r="AC1" s="18">
+      <c r="AC1" s="17">
         <v>1998</v>
       </c>
-      <c r="AD1" s="16">
+      <c r="AD1" s="15">
         <v>1999</v>
       </c>
-      <c r="AE1" s="17">
+      <c r="AE1" s="16">
         <v>2000</v>
       </c>
-      <c r="AF1" s="17">
+      <c r="AF1" s="16">
         <v>2001</v>
       </c>
-      <c r="AG1" s="17">
+      <c r="AG1" s="16">
         <v>2002</v>
       </c>
-      <c r="AH1" s="18">
+      <c r="AH1" s="17">
         <v>2003</v>
       </c>
-      <c r="AI1" s="16">
+      <c r="AI1" s="15">
         <v>2004</v>
       </c>
-      <c r="AJ1" s="17">
+      <c r="AJ1" s="16">
         <v>2005</v>
       </c>
-      <c r="AK1" s="17">
+      <c r="AK1" s="16">
         <v>2006</v>
       </c>
-      <c r="AL1" s="17">
+      <c r="AL1" s="16">
         <v>2007</v>
       </c>
-      <c r="AM1" s="18">
+      <c r="AM1" s="17">
         <v>2008</v>
       </c>
-      <c r="AN1" s="16">
+      <c r="AN1" s="15">
         <v>2009</v>
       </c>
-      <c r="AO1" s="17">
+      <c r="AO1" s="16">
         <v>2010</v>
       </c>
-      <c r="AP1" s="17">
+      <c r="AP1" s="16">
         <v>2011</v>
       </c>
-      <c r="AQ1" s="17">
+      <c r="AQ1" s="16">
         <v>2012</v>
       </c>
-      <c r="AR1" s="18">
+      <c r="AR1" s="17">
         <v>2013</v>
       </c>
-      <c r="AS1" s="16">
+      <c r="AS1" s="15">
         <v>2014</v>
       </c>
-      <c r="AT1" s="17">
+      <c r="AT1" s="16">
         <v>2015</v>
       </c>
-      <c r="AU1" s="17">
+      <c r="AU1" s="16">
         <v>2016</v>
       </c>
-      <c r="AV1" s="18">
+      <c r="AV1" s="17">
         <v>2017</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="4"/>
       <c r="G2" s="7"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="20"/>
       <c r="K2" s="4"/>
       <c r="L2" s="7"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="21"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="20"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="31"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="25"/>
       <c r="U2" s="2"/>
       <c r="V2" s="6"/>
       <c r="W2" s="2"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="31"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="25"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="6"/>
       <c r="AB2" s="2"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="31"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="25"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="6"/>
       <c r="AG2" s="2"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="31"/>
+      <c r="AH2" s="24"/>
+      <c r="AI2" s="25"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="6"/>
       <c r="AL2" s="2"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="31"/>
+      <c r="AM2" s="24"/>
+      <c r="AN2" s="25"/>
       <c r="AO2" s="2"/>
       <c r="AP2" s="6"/>
       <c r="AQ2" s="2"/>
-      <c r="AR2" s="28"/>
-      <c r="AS2" s="31"/>
+      <c r="AR2" s="24"/>
+      <c r="AS2" s="25"/>
       <c r="AT2" s="2"/>
       <c r="AU2" s="6"/>
-      <c r="AV2" s="28"/>
+      <c r="AV2" s="24"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="21"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="20"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="31"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="25"/>
       <c r="U3" s="2"/>
       <c r="V3" s="10"/>
       <c r="W3" s="2"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="31"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="25"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="10"/>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="31"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="25"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="10"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="31"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="25"/>
       <c r="AJ3" s="2"/>
       <c r="AK3" s="10"/>
       <c r="AL3" s="2"/>
-      <c r="AM3" s="28"/>
-      <c r="AN3" s="31"/>
+      <c r="AM3" s="24"/>
+      <c r="AN3" s="25"/>
       <c r="AO3" s="2"/>
       <c r="AP3" s="10"/>
       <c r="AQ3" s="2"/>
-      <c r="AR3" s="28"/>
-      <c r="AS3" s="31"/>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="25"/>
       <c r="AT3" s="2"/>
       <c r="AU3" s="10"/>
-      <c r="AV3" s="28"/>
+      <c r="AV3" s="24"/>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="21"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="20"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="31"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="25"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="31"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="25"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="31"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="25"/>
       <c r="AE4" s="2"/>
       <c r="AF4" s="11"/>
       <c r="AG4" s="11"/>
-      <c r="AH4" s="33"/>
-      <c r="AI4" s="36"/>
+      <c r="AH4" s="26"/>
+      <c r="AI4" s="29"/>
       <c r="AJ4" s="11"/>
       <c r="AK4" s="11"/>
       <c r="AL4" s="11"/>
-      <c r="AM4" s="33"/>
-      <c r="AN4" s="36"/>
+      <c r="AM4" s="26"/>
+      <c r="AN4" s="29"/>
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
       <c r="AQ4" s="11"/>
-      <c r="AR4" s="33"/>
-      <c r="AS4" s="36"/>
+      <c r="AR4" s="26"/>
+      <c r="AS4" s="29"/>
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
-      <c r="AV4" s="28"/>
+      <c r="AV4" s="24"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="20"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="21"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="20"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="31"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="25"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
-      <c r="X5" s="28"/>
-      <c r="Y5" s="31"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="25"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
-      <c r="AC5" s="28"/>
-      <c r="AD5" s="31"/>
+      <c r="AC5" s="24"/>
+      <c r="AD5" s="25"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="13"/>
       <c r="AG5" s="13"/>
-      <c r="AH5" s="34"/>
-      <c r="AI5" s="37"/>
+      <c r="AH5" s="27"/>
+      <c r="AI5" s="30"/>
       <c r="AJ5" s="13"/>
       <c r="AK5" s="13"/>
       <c r="AL5" s="13"/>
-      <c r="AM5" s="34"/>
-      <c r="AN5" s="37"/>
+      <c r="AM5" s="27"/>
+      <c r="AN5" s="30"/>
       <c r="AO5" s="13"/>
       <c r="AP5" s="13"/>
       <c r="AQ5" s="13"/>
-      <c r="AR5" s="34"/>
-      <c r="AS5" s="37"/>
+      <c r="AR5" s="27"/>
+      <c r="AS5" s="30"/>
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
-      <c r="AV5" s="28"/>
+      <c r="AV5" s="24"/>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="21"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="21"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="20"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="31"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="25"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="31"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="25"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
-      <c r="AC6" s="28"/>
-      <c r="AD6" s="31"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="25"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="12"/>
       <c r="AG6" s="12"/>
-      <c r="AH6" s="35"/>
-      <c r="AI6" s="38"/>
+      <c r="AH6" s="28"/>
+      <c r="AI6" s="31"/>
       <c r="AJ6" s="12"/>
       <c r="AK6" s="12"/>
       <c r="AL6" s="12"/>
-      <c r="AM6" s="35"/>
-      <c r="AN6" s="38"/>
+      <c r="AM6" s="28"/>
+      <c r="AN6" s="31"/>
       <c r="AO6" s="12"/>
       <c r="AP6" s="12"/>
       <c r="AQ6" s="12"/>
-      <c r="AR6" s="35"/>
-      <c r="AS6" s="31"/>
+      <c r="AR6" s="28"/>
+      <c r="AS6" s="25"/>
       <c r="AT6" s="2"/>
       <c r="AU6" s="2"/>
-      <c r="AV6" s="28"/>
+      <c r="AV6" s="24"/>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="4"/>
       <c r="G7" s="8"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="20"/>
       <c r="K7" s="4"/>
       <c r="L7" s="8"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="21"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="20"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="31"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="25"/>
       <c r="U7" s="2"/>
       <c r="V7" s="9"/>
       <c r="W7" s="2"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="31"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="25"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="9"/>
       <c r="AB7" s="2"/>
-      <c r="AC7" s="28"/>
-      <c r="AD7" s="31"/>
+      <c r="AC7" s="24"/>
+      <c r="AD7" s="25"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="9"/>
       <c r="AG7" s="2"/>
-      <c r="AH7" s="28"/>
-      <c r="AI7" s="31"/>
+      <c r="AH7" s="24"/>
+      <c r="AI7" s="25"/>
       <c r="AJ7" s="2"/>
       <c r="AK7" s="9"/>
       <c r="AL7" s="2"/>
-      <c r="AM7" s="28"/>
-      <c r="AN7" s="31"/>
+      <c r="AM7" s="24"/>
+      <c r="AN7" s="25"/>
       <c r="AO7" s="2"/>
       <c r="AP7" s="9"/>
       <c r="AQ7" s="2"/>
-      <c r="AR7" s="28"/>
-      <c r="AS7" s="31"/>
+      <c r="AR7" s="24"/>
+      <c r="AS7" s="25"/>
       <c r="AT7" s="2"/>
       <c r="AU7" s="9"/>
-      <c r="AV7" s="28"/>
+      <c r="AV7" s="24"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="22"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="22"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="22"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="22"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="22"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
-      <c r="AC8" s="24"/>
-      <c r="AD8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="22"/>
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
-      <c r="AH8" s="24"/>
-      <c r="AI8" s="23"/>
+      <c r="AH8" s="23"/>
+      <c r="AI8" s="22"/>
       <c r="AJ8" s="3"/>
       <c r="AK8" s="3"/>
       <c r="AL8" s="3"/>
-      <c r="AM8" s="24"/>
-      <c r="AN8" s="23"/>
+      <c r="AM8" s="23"/>
+      <c r="AN8" s="22"/>
       <c r="AO8" s="3"/>
       <c r="AP8" s="3"/>
       <c r="AQ8" s="3"/>
-      <c r="AR8" s="24"/>
-      <c r="AS8" s="23"/>
+      <c r="AR8" s="23"/>
+      <c r="AS8" s="22"/>
       <c r="AT8" s="3"/>
       <c r="AU8" s="3"/>
-      <c r="AV8" s="24"/>
+      <c r="AV8" s="23"/>
     </row>
     <row r="9" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="32"/>
-      <c r="Z9" s="29"/>
-      <c r="AA9" s="29"/>
-      <c r="AB9" s="29"/>
-      <c r="AC9" s="30"/>
-      <c r="AD9" s="32"/>
-      <c r="AE9" s="29"/>
-      <c r="AF9" s="29"/>
-      <c r="AG9" s="29"/>
-      <c r="AH9" s="30"/>
-      <c r="AI9" s="32"/>
-      <c r="AJ9" s="29"/>
-      <c r="AK9" s="29"/>
-      <c r="AL9" s="29"/>
-      <c r="AM9" s="30"/>
-      <c r="AN9" s="32"/>
-      <c r="AO9" s="29"/>
-      <c r="AP9" s="39"/>
-      <c r="AQ9" s="29"/>
-      <c r="AR9" s="30"/>
-      <c r="AS9" s="32"/>
-      <c r="AT9" s="29"/>
-      <c r="AU9" s="29"/>
-      <c r="AV9" s="30"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="36"/>
+      <c r="Y9" s="37"/>
+      <c r="Z9" s="35"/>
+      <c r="AA9" s="35"/>
+      <c r="AB9" s="35"/>
+      <c r="AC9" s="36"/>
+      <c r="AD9" s="37"/>
+      <c r="AE9" s="35"/>
+      <c r="AF9" s="35"/>
+      <c r="AG9" s="35"/>
+      <c r="AH9" s="36"/>
+      <c r="AI9" s="37"/>
+      <c r="AJ9" s="35"/>
+      <c r="AK9" s="35"/>
+      <c r="AL9" s="35"/>
+      <c r="AM9" s="36"/>
+      <c r="AN9" s="37"/>
+      <c r="AO9" s="35"/>
+      <c r="AP9" s="38"/>
+      <c r="AQ9" s="35"/>
+      <c r="AR9" s="36"/>
+      <c r="AS9" s="37"/>
+      <c r="AT9" s="35"/>
+      <c r="AU9" s="35"/>
+      <c r="AV9" s="36"/>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+    <row r="10" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="50" t="s">
         <v>9</v>
       </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="40"/>
       <c r="Q10" s="41"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="46"/>
+      <c r="U10" s="40"/>
       <c r="V10" s="41"/>
+      <c r="W10" s="40"/>
+      <c r="X10" s="42"/>
+      <c r="Y10" s="46"/>
+      <c r="Z10" s="40"/>
       <c r="AA10" s="41"/>
+      <c r="AB10" s="40"/>
+      <c r="AC10" s="42"/>
+      <c r="AD10" s="46"/>
+      <c r="AE10" s="40"/>
       <c r="AF10" s="41"/>
+      <c r="AG10" s="40"/>
+      <c r="AH10" s="42"/>
+      <c r="AI10" s="46"/>
+      <c r="AJ10" s="40"/>
       <c r="AK10" s="41"/>
+      <c r="AL10" s="40"/>
+      <c r="AM10" s="42"/>
+      <c r="AN10" s="46"/>
+      <c r="AO10" s="40"/>
       <c r="AP10" s="41"/>
+      <c r="AQ10" s="40"/>
+      <c r="AR10" s="42"/>
+      <c r="AS10" s="45"/>
+      <c r="AT10" s="40"/>
       <c r="AU10" s="41"/>
+      <c r="AV10" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>